<commit_message>
Finalized UI and backedn logic
</commit_message>
<xml_diff>
--- a/backend/excel/medicine-db.xlsx
+++ b/backend/excel/medicine-db.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -28,79 +28,139 @@
     <t>Balance</t>
   </si>
   <si>
+    <t>imageURL</t>
+  </si>
+  <si>
     <t>Paracetamol</t>
   </si>
   <si>
     <t>Tablet</t>
   </si>
   <si>
+    <t>https://tgp.com.ph/3647/paracetamol-500mg-tablet.jpg</t>
+  </si>
+  <si>
     <t>Amoxicillin</t>
   </si>
   <si>
     <t>Capsule</t>
   </si>
   <si>
+    <t>https://medias.watsons.com.ph/publishing/WTCPH-10030303-front-zoom.jpg?version=1721934643</t>
+  </si>
+  <si>
     <t>Ibuprofen</t>
   </si>
   <si>
     <t>Syrup</t>
   </si>
   <si>
+    <t>https://mpfshstrg.blob.core.windows.net/mpf-uat-drug-resources/SG/packshot/Brufen6001PPS0.JPG</t>
+  </si>
+  <si>
     <t>Cetrizine</t>
   </si>
   <si>
+    <t>https://wholesale.farmasiehsan.com.my/wp-content/uploads/2022/11/CETIRIZINE-10MG.png</t>
+  </si>
+  <si>
     <t>Metformin</t>
   </si>
   <si>
+    <t>https://images.ctfassets.net/4w8qvp17lo47/6vXaH4Y5Gw6AMEmASwGkc6/e6ff962a82811e4d160cc2d5c0d8b3cb/metformin-antidiabetic-tablets-science-photo-library.jpg</t>
+  </si>
+  <si>
     <t>Omeprazole</t>
   </si>
   <si>
+    <t>https://medias.watsons.com.ph/publishing/WTCPH-50026139-front-zoom.jpg?version=1721934859</t>
+  </si>
+  <si>
     <t>Aspirin</t>
   </si>
   <si>
+    <t>https://5.imimg.com/data5/SELLER/Default/2023/7/330506870/UM/GZ/QO/135658020/aspirin-dispersible-tablets.jpg</t>
+  </si>
+  <si>
     <t>Atorvastatin</t>
   </si>
   <si>
+    <t>https://medias.watsons.com.ph/publishing/WTCPH-10090918-front-zoom.jpg?version=1721934590</t>
+  </si>
+  <si>
     <t>Salbutamol</t>
   </si>
   <si>
     <t>Inhaler</t>
   </si>
   <si>
+    <t>https://image.made-in-china.com/202f0j00pqglAcOskjfo/Salbutamol-Sulfate-Aerosol-100mcg-Dose.webp</t>
+  </si>
+  <si>
     <t>Diclofenac</t>
   </si>
   <si>
     <t>Gel</t>
   </si>
   <si>
+    <t>https://www.dottortili.com/cdn/shop/files/VoltarenEmulgel1_60g.jpg?v=1695907656</t>
+  </si>
+  <si>
     <t>Loratadine</t>
   </si>
   <si>
+    <t>https://images.apollo247.in/pub/media/catalog/product/l/o/lor0635_3.jpg?tr=q-80,f-webp,w-400,dpr-3,c-at_max%201200w</t>
+  </si>
+  <si>
     <t>Ranitidine</t>
   </si>
   <si>
+    <t>https://www.xalmeds.com/cdn/shop/files/IMG_6478.jpg?v=1698647526</t>
+  </si>
+  <si>
     <t>Doxycycline</t>
   </si>
   <si>
+    <t>https://image.made-in-china.com/2f0j00cqOhjCFKevUm/Doxycycline-Hyclate-Capsules-100mg-GMP-Medicine.webp</t>
+  </si>
+  <si>
     <t>Prednisolone</t>
   </si>
   <si>
+    <t>https://medias.watsons.com.my/publishing/WTCMY-1011756-back-zoom.jpg?version=1722634216</t>
+  </si>
+  <si>
     <t>Ciprofloxacin</t>
   </si>
   <si>
+    <t>https://www.actizapharma.com/wp-content/uploads/2024/01/ciprofloxacin_500mg_tablet_1.webp</t>
+  </si>
+  <si>
     <t>Levothyroxine</t>
   </si>
   <si>
+    <t>https://medias.watsons.com.ph/publishing/WTCPH-10003233-front-zoom.jpg?version=1721934883</t>
+  </si>
+  <si>
     <t>Metoprolol</t>
   </si>
   <si>
+    <t>https://medias.watsons.com.ph/publishing/WTCPH-10090916-front-zoom.jpg?version=1721934592</t>
+  </si>
+  <si>
     <t>Insulin</t>
   </si>
   <si>
     <t>Injection</t>
   </si>
   <si>
+    <t>https://www.cphi-online.com/46/product/129/68/72/Mysulin%20R%20Product%20Packshot%20.png</t>
+  </si>
+  <si>
     <t>Hydrochlorothiazide</t>
+  </si>
+  <si>
+    <t>https://www.xalmeds.com/cdn/shop/files/IMG_6307_c88c200b-0d59-4742-88c4-1072abb6012e_1445x.jpg?v=1728121605</t>
   </si>
 </sst>
 </file>
@@ -118,7 +178,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -150,15 +210,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -166,6 +226,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,7 +532,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -478,10 +541,11 @@
     <col min="1" max="1" style="4" width="9.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="16.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="72.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,271 +558,331 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1">
+        <v>50</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>200</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="D2" s="3">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>150</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1">
+        <v>120</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>250</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>180</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1">
+        <v>60</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1">
+        <v>40</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>130</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="E13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3">
-        <v>150</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3">
-        <v>120</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>250</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="D14" s="1">
+        <v>110</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3">
-        <v>180</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1">
+        <v>75</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>85</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="D10" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1">
+        <v>95</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>105</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="D11" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="1">
+        <v>70</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="3">
-        <v>130</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3">
-        <v>110</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="3">
-        <v>75</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="3">
-        <v>85</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="3">
-        <v>95</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="3">
-        <v>105</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
       <c r="B20" s="2" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="3">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1">
         <v>55</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>